<commit_message>
updata font and ui
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1499</v>
+        <v>1300</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">

</xml_diff>